<commit_message>
Fixing classes form json-schema generation
</commit_message>
<xml_diff>
--- a/src/test/resources/rules.xlsx
+++ b/src/test/resources/rules.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="73">
   <si>
     <t>RuleSet</t>
   </si>
@@ -67,9 +67,6 @@
   </si>
   <si>
     <t>getFirstName() != null &amp;&amp; getFirstName() $param  ""</t>
-  </si>
-  <si>
-    <t>RuleLogging.log("$1", "Rule - $2 - fired");</t>
   </si>
   <si>
     <t>Catalogue</t>
@@ -239,9 +236,18 @@
     <t>$person : Person</t>
   </si>
   <si>
-    <t>RuleMessageError errorEn = new RuleMessageError("$3", "$4", "$5", "$6", "$1", "$2", null);                
+    <t>RuleMessageError errorEn = new RuleMessageError("$3", "$4", "$5", "$6", "$1", "$2",$10);                
 insert( errorEn );
-RuleMessageError errorEs = new RuleMessageError("$7", "$8", "$9", "$10", "$1", "$2", null);        
+RuleMessageError errorEs = new RuleMessageError("$7", "$8", "$9", "$10", "$1", "$2",$10);        
+insert( errorEs );</t>
+  </si>
+  <si>
+    <t>RuleLogging.log("$1", "Rule - $2 - fired");</t>
+  </si>
+  <si>
+    <t>RuleMessageError errorEn = new RuleMessageError("$3", "$4", "$5", "$6", "$1", "$2",$10);                
+insert( errorEn );
+RuleMessageError errorEs = new RuleMessageError("$3", "$4", "$5", "$6", "$1", "$2",$10);        
 insert( errorEs );</t>
   </si>
 </sst>
@@ -973,6 +979,11 @@
     <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -981,16 +992,11 @@
     <xf numFmtId="0" fontId="8" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1498,8 +1504,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AP1000"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="AA11" workbookViewId="0">
-      <selection activeCell="AG17" sqref="AG17"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="AF15" workbookViewId="0">
+      <selection activeCell="AG21" sqref="AG21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -1526,7 +1532,7 @@
     <col min="29" max="29" width="26.5546875" customWidth="1"/>
     <col min="30" max="30" width="45.5546875" customWidth="1"/>
     <col min="31" max="31" width="33.109375" customWidth="1"/>
-    <col min="32" max="32" width="27.88671875" customWidth="1"/>
+    <col min="32" max="32" width="38.6640625" customWidth="1"/>
     <col min="33" max="33" width="44.33203125" customWidth="1"/>
     <col min="34" max="34" width="20" customWidth="1"/>
     <col min="35" max="35" width="21" customWidth="1"/>
@@ -1571,7 +1577,7 @@
         <v>0</v>
       </c>
       <c r="AD1" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AE1" s="5"/>
       <c r="AF1" s="5"/>
@@ -1619,7 +1625,7 @@
         <v>1</v>
       </c>
       <c r="AD2" s="70" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="AE2" s="5"/>
       <c r="AF2" s="5"/>
@@ -1680,45 +1686,45 @@
     </row>
     <row r="4" spans="1:42" ht="21">
       <c r="A4" s="3"/>
-      <c r="B4" s="71" t="s">
+      <c r="B4" s="74" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="72"/>
-      <c r="D4" s="72"/>
-      <c r="E4" s="72"/>
-      <c r="F4" s="72"/>
-      <c r="G4" s="72"/>
-      <c r="H4" s="72"/>
-      <c r="I4" s="72"/>
-      <c r="J4" s="72"/>
-      <c r="K4" s="72"/>
-      <c r="L4" s="72"/>
-      <c r="M4" s="72"/>
-      <c r="N4" s="72"/>
-      <c r="O4" s="72"/>
-      <c r="P4" s="72"/>
-      <c r="Q4" s="72"/>
-      <c r="R4" s="72"/>
-      <c r="S4" s="72"/>
-      <c r="T4" s="72"/>
-      <c r="U4" s="72"/>
-      <c r="V4" s="72"/>
-      <c r="W4" s="72"/>
-      <c r="X4" s="72"/>
-      <c r="Y4" s="72"/>
-      <c r="Z4" s="72"/>
-      <c r="AA4" s="72"/>
-      <c r="AB4" s="72"/>
-      <c r="AC4" s="72"/>
-      <c r="AD4" s="72"/>
-      <c r="AE4" s="72"/>
-      <c r="AF4" s="72"/>
-      <c r="AG4" s="72"/>
-      <c r="AH4" s="72"/>
-      <c r="AI4" s="72"/>
-      <c r="AJ4" s="72"/>
-      <c r="AK4" s="72"/>
-      <c r="AL4" s="73"/>
+      <c r="C4" s="75"/>
+      <c r="D4" s="75"/>
+      <c r="E4" s="75"/>
+      <c r="F4" s="75"/>
+      <c r="G4" s="75"/>
+      <c r="H4" s="75"/>
+      <c r="I4" s="75"/>
+      <c r="J4" s="75"/>
+      <c r="K4" s="75"/>
+      <c r="L4" s="75"/>
+      <c r="M4" s="75"/>
+      <c r="N4" s="75"/>
+      <c r="O4" s="75"/>
+      <c r="P4" s="75"/>
+      <c r="Q4" s="75"/>
+      <c r="R4" s="75"/>
+      <c r="S4" s="75"/>
+      <c r="T4" s="75"/>
+      <c r="U4" s="75"/>
+      <c r="V4" s="75"/>
+      <c r="W4" s="75"/>
+      <c r="X4" s="75"/>
+      <c r="Y4" s="75"/>
+      <c r="Z4" s="75"/>
+      <c r="AA4" s="75"/>
+      <c r="AB4" s="75"/>
+      <c r="AC4" s="75"/>
+      <c r="AD4" s="75"/>
+      <c r="AE4" s="75"/>
+      <c r="AF4" s="75"/>
+      <c r="AG4" s="75"/>
+      <c r="AH4" s="75"/>
+      <c r="AI4" s="75"/>
+      <c r="AJ4" s="75"/>
+      <c r="AK4" s="75"/>
+      <c r="AL4" s="76"/>
       <c r="AM4" s="3"/>
       <c r="AN4" s="3"/>
       <c r="AO4" s="3"/>
@@ -1726,33 +1732,33 @@
     <row r="5" spans="1:42" ht="15" customHeight="1">
       <c r="A5" s="10"/>
       <c r="B5" s="11"/>
-      <c r="C5" s="74" t="s">
+      <c r="C5" s="77" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="72"/>
-      <c r="E5" s="72"/>
-      <c r="F5" s="72"/>
-      <c r="G5" s="72"/>
-      <c r="H5" s="72"/>
-      <c r="I5" s="72"/>
-      <c r="J5" s="72"/>
-      <c r="K5" s="72"/>
-      <c r="L5" s="72"/>
-      <c r="M5" s="72"/>
-      <c r="N5" s="72"/>
-      <c r="O5" s="72"/>
-      <c r="P5" s="72"/>
-      <c r="Q5" s="72"/>
-      <c r="R5" s="72"/>
-      <c r="S5" s="72"/>
-      <c r="T5" s="72"/>
-      <c r="U5" s="72"/>
-      <c r="V5" s="72"/>
-      <c r="W5" s="72"/>
-      <c r="X5" s="72"/>
-      <c r="Y5" s="72"/>
-      <c r="Z5" s="72"/>
-      <c r="AA5" s="73"/>
+      <c r="D5" s="75"/>
+      <c r="E5" s="75"/>
+      <c r="F5" s="75"/>
+      <c r="G5" s="75"/>
+      <c r="H5" s="75"/>
+      <c r="I5" s="75"/>
+      <c r="J5" s="75"/>
+      <c r="K5" s="75"/>
+      <c r="L5" s="75"/>
+      <c r="M5" s="75"/>
+      <c r="N5" s="75"/>
+      <c r="O5" s="75"/>
+      <c r="P5" s="75"/>
+      <c r="Q5" s="75"/>
+      <c r="R5" s="75"/>
+      <c r="S5" s="75"/>
+      <c r="T5" s="75"/>
+      <c r="U5" s="75"/>
+      <c r="V5" s="75"/>
+      <c r="W5" s="75"/>
+      <c r="X5" s="75"/>
+      <c r="Y5" s="75"/>
+      <c r="Z5" s="75"/>
+      <c r="AA5" s="76"/>
       <c r="AB5" s="12"/>
       <c r="AC5" s="13" t="s">
         <v>4</v>
@@ -1812,20 +1818,20 @@
       <c r="U6" s="22"/>
       <c r="V6" s="22"/>
       <c r="W6" s="12"/>
-      <c r="X6" s="77" t="s">
+      <c r="X6" s="78" t="s">
         <v>12</v>
       </c>
-      <c r="Y6" s="78"/>
-      <c r="Z6" s="77" t="s">
+      <c r="Y6" s="79"/>
+      <c r="Z6" s="78" t="s">
         <v>13</v>
       </c>
-      <c r="AA6" s="79"/>
+      <c r="AA6" s="80"/>
       <c r="AB6" s="23"/>
       <c r="AC6" s="24"/>
-      <c r="AD6" s="75" t="s">
-        <v>70</v>
-      </c>
-      <c r="AE6" s="76"/>
+      <c r="AD6" s="71" t="s">
+        <v>69</v>
+      </c>
+      <c r="AE6" s="73"/>
       <c r="AF6" s="25"/>
       <c r="AG6" s="26"/>
       <c r="AH6" s="20"/>
@@ -1874,10 +1880,10 @@
         <v>15</v>
       </c>
       <c r="AF7" s="35" t="s">
+        <v>72</v>
+      </c>
+      <c r="AG7" s="36" t="s">
         <v>71</v>
-      </c>
-      <c r="AG7" s="36" t="s">
-        <v>16</v>
       </c>
       <c r="AH7" s="20"/>
       <c r="AI7" s="20"/>
@@ -1892,7 +1898,7 @@
       <c r="A8" s="37"/>
       <c r="B8" s="38"/>
       <c r="C8" s="39" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D8" s="40"/>
       <c r="E8" s="40"/>
@@ -1905,7 +1911,7 @@
       <c r="L8" s="40"/>
       <c r="M8" s="40"/>
       <c r="N8" s="39" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="O8" s="40"/>
       <c r="P8" s="40"/>
@@ -1914,54 +1920,54 @@
       <c r="S8" s="40"/>
       <c r="T8" s="40"/>
       <c r="U8" s="41" t="s">
+        <v>18</v>
+      </c>
+      <c r="V8" s="41" t="s">
         <v>19</v>
-      </c>
-      <c r="V8" s="41" t="s">
-        <v>20</v>
       </c>
       <c r="W8" s="42"/>
       <c r="X8" s="43" t="s">
+        <v>20</v>
+      </c>
+      <c r="Y8" s="44" t="s">
         <v>21</v>
       </c>
-      <c r="Y8" s="44" t="s">
+      <c r="Z8" s="45" t="s">
         <v>22</v>
       </c>
-      <c r="Z8" s="45" t="s">
+      <c r="AA8" s="46" t="s">
         <v>23</v>
-      </c>
-      <c r="AA8" s="46" t="s">
-        <v>24</v>
       </c>
       <c r="AB8" s="47"/>
       <c r="AC8" s="48" t="s">
+        <v>24</v>
+      </c>
+      <c r="AD8" s="49" t="s">
         <v>25</v>
       </c>
-      <c r="AD8" s="49" t="s">
+      <c r="AE8" s="49" t="s">
         <v>26</v>
       </c>
-      <c r="AE8" s="49" t="s">
+      <c r="AF8" s="50" t="s">
         <v>27</v>
       </c>
-      <c r="AF8" s="50" t="s">
+      <c r="AG8" s="50" t="s">
         <v>28</v>
       </c>
-      <c r="AG8" s="50" t="s">
+      <c r="AH8" s="51" t="s">
         <v>29</v>
       </c>
-      <c r="AH8" s="51" t="s">
+      <c r="AI8" s="52" t="s">
         <v>30</v>
       </c>
-      <c r="AI8" s="52" t="s">
+      <c r="AJ8" s="52" t="s">
         <v>31</v>
       </c>
-      <c r="AJ8" s="52" t="s">
+      <c r="AK8" s="52" t="s">
         <v>32</v>
       </c>
-      <c r="AK8" s="52" t="s">
+      <c r="AL8" s="51" t="s">
         <v>33</v>
-      </c>
-      <c r="AL8" s="51" t="s">
-        <v>34</v>
       </c>
       <c r="AM8" s="3"/>
       <c r="AN8" s="3"/>
@@ -1984,7 +1990,7 @@
       <c r="L9" s="54"/>
       <c r="M9" s="54"/>
       <c r="N9" s="55" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="O9" s="56"/>
       <c r="P9" s="56"/>
@@ -1997,20 +2003,20 @@
         <v>firstName</v>
       </c>
       <c r="V9" s="56" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="W9" s="57"/>
       <c r="X9" s="58" t="s">
+        <v>36</v>
+      </c>
+      <c r="Y9" s="58" t="s">
         <v>37</v>
       </c>
-      <c r="Y9" s="58" t="s">
+      <c r="Z9" s="58" t="s">
         <v>38</v>
       </c>
-      <c r="Z9" s="58" t="s">
+      <c r="AA9" s="58" t="s">
         <v>39</v>
-      </c>
-      <c r="AA9" s="58" t="s">
-        <v>40</v>
       </c>
       <c r="AB9" s="59"/>
       <c r="AC9" s="60" t="str">
@@ -2018,7 +2024,7 @@
         <v>Person's first name cannot be null</v>
       </c>
       <c r="AD9" s="61" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="AE9" s="61"/>
       <c r="AF9" s="62" t="str">
@@ -2030,7 +2036,7 @@
         <v>ERROR,Person's first name cannot be null</v>
       </c>
       <c r="AH9" s="63" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="AI9" s="64" t="str">
         <f t="shared" ref="AI9:AI10" si="3">U9</f>
@@ -2044,13 +2050,13 @@
         <v>true</v>
       </c>
       <c r="AL9" s="63" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="AM9" s="4"/>
       <c r="AN9" s="4"/>
       <c r="AO9" s="4"/>
     </row>
-    <row r="10" spans="1:42" ht="172.8">
+    <row r="10" spans="1:42" ht="115.2">
       <c r="A10" s="4"/>
       <c r="B10" s="53"/>
       <c r="C10" s="54">
@@ -2067,7 +2073,7 @@
       <c r="L10" s="54"/>
       <c r="M10" s="54"/>
       <c r="N10" s="55" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="O10" s="56"/>
       <c r="P10" s="56"/>
@@ -2080,20 +2086,20 @@
         <v>firstName</v>
       </c>
       <c r="V10" s="56" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="W10" s="57"/>
       <c r="X10" s="58" t="s">
+        <v>42</v>
+      </c>
+      <c r="Y10" s="58" t="s">
         <v>43</v>
       </c>
-      <c r="Y10" s="58" t="s">
+      <c r="Z10" s="58" t="s">
         <v>44</v>
       </c>
-      <c r="Z10" s="58" t="s">
+      <c r="AA10" s="58" t="s">
         <v>45</v>
-      </c>
-      <c r="AA10" s="58" t="s">
-        <v>46</v>
       </c>
       <c r="AB10" s="59"/>
       <c r="AC10" s="60" t="str">
@@ -2102,10 +2108,10 @@
       </c>
       <c r="AD10" s="61"/>
       <c r="AE10" s="61" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="AF10" s="62" t="str">
-        <f t="shared" ref="AF10" si="5">CONCATENATE( "person",",",U10,",",$X$6,",",C10," [",U10,"] - ",X10,",",X10,",",Y10,",", $Z$6,",",C10," [",U10,"] - ",Z10,",",Z10,",",AA10,",","$person.getFirstName()")</f>
+        <f>CONCATENATE( "person",",",U10,",",$X$6,",",C10," [",U10,"] - ",X10,",",X10,",",Y10,",", $Z$6,",",C10," [",U10,"] - ",Z10,",",Z10,",",AA10,",","$person.getFirstName()")</f>
         <v>person,firstName,en,1 [firstName] - Person's first name cannot be empty,Person's first name cannot be empty,A name with some value different than empty,es,1 [firstName] - El primer nombre de la persona no pude ser vacío,El primer nombre de la persona no pude ser vacío,Un nombre con algún valor diferente de vacío,$person.getFirstName()</v>
       </c>
       <c r="AG10" s="58" t="str">
@@ -2113,7 +2119,7 @@
         <v>ERROR,Person's first name cannot be empty</v>
       </c>
       <c r="AH10" s="63" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="AI10" s="64" t="str">
         <f t="shared" si="3"/>
@@ -2136,79 +2142,79 @@
     </row>
     <row r="11" spans="1:42" ht="21">
       <c r="A11" s="3"/>
-      <c r="B11" s="71" t="s">
-        <v>47</v>
-      </c>
-      <c r="C11" s="72"/>
-      <c r="D11" s="72"/>
-      <c r="E11" s="72"/>
-      <c r="F11" s="72"/>
-      <c r="G11" s="72"/>
-      <c r="H11" s="72"/>
-      <c r="I11" s="72"/>
-      <c r="J11" s="72"/>
-      <c r="K11" s="72"/>
-      <c r="L11" s="72"/>
-      <c r="M11" s="72"/>
-      <c r="N11" s="72"/>
-      <c r="O11" s="72"/>
-      <c r="P11" s="72"/>
-      <c r="Q11" s="72"/>
-      <c r="R11" s="72"/>
-      <c r="S11" s="72"/>
-      <c r="T11" s="72"/>
-      <c r="U11" s="72"/>
-      <c r="V11" s="72"/>
-      <c r="W11" s="72"/>
-      <c r="X11" s="72"/>
-      <c r="Y11" s="72"/>
-      <c r="Z11" s="72"/>
-      <c r="AA11" s="72"/>
-      <c r="AB11" s="72"/>
-      <c r="AC11" s="72"/>
-      <c r="AD11" s="72"/>
-      <c r="AE11" s="72"/>
-      <c r="AF11" s="72"/>
-      <c r="AG11" s="72"/>
-      <c r="AH11" s="72"/>
-      <c r="AI11" s="72"/>
-      <c r="AJ11" s="72"/>
-      <c r="AK11" s="72"/>
-      <c r="AL11" s="72"/>
-      <c r="AM11" s="73"/>
+      <c r="B11" s="74" t="s">
+        <v>46</v>
+      </c>
+      <c r="C11" s="75"/>
+      <c r="D11" s="75"/>
+      <c r="E11" s="75"/>
+      <c r="F11" s="75"/>
+      <c r="G11" s="75"/>
+      <c r="H11" s="75"/>
+      <c r="I11" s="75"/>
+      <c r="J11" s="75"/>
+      <c r="K11" s="75"/>
+      <c r="L11" s="75"/>
+      <c r="M11" s="75"/>
+      <c r="N11" s="75"/>
+      <c r="O11" s="75"/>
+      <c r="P11" s="75"/>
+      <c r="Q11" s="75"/>
+      <c r="R11" s="75"/>
+      <c r="S11" s="75"/>
+      <c r="T11" s="75"/>
+      <c r="U11" s="75"/>
+      <c r="V11" s="75"/>
+      <c r="W11" s="75"/>
+      <c r="X11" s="75"/>
+      <c r="Y11" s="75"/>
+      <c r="Z11" s="75"/>
+      <c r="AA11" s="75"/>
+      <c r="AB11" s="75"/>
+      <c r="AC11" s="75"/>
+      <c r="AD11" s="75"/>
+      <c r="AE11" s="75"/>
+      <c r="AF11" s="75"/>
+      <c r="AG11" s="75"/>
+      <c r="AH11" s="75"/>
+      <c r="AI11" s="75"/>
+      <c r="AJ11" s="75"/>
+      <c r="AK11" s="75"/>
+      <c r="AL11" s="75"/>
+      <c r="AM11" s="76"/>
       <c r="AN11" s="3"/>
       <c r="AO11" s="3"/>
     </row>
     <row r="12" spans="1:42" ht="15" customHeight="1">
       <c r="A12" s="10"/>
       <c r="B12" s="11"/>
-      <c r="C12" s="74" t="s">
+      <c r="C12" s="77" t="s">
         <v>3</v>
       </c>
-      <c r="D12" s="72"/>
-      <c r="E12" s="72"/>
-      <c r="F12" s="72"/>
-      <c r="G12" s="72"/>
-      <c r="H12" s="72"/>
-      <c r="I12" s="72"/>
-      <c r="J12" s="72"/>
-      <c r="K12" s="72"/>
-      <c r="L12" s="72"/>
-      <c r="M12" s="72"/>
-      <c r="N12" s="72"/>
-      <c r="O12" s="72"/>
-      <c r="P12" s="72"/>
-      <c r="Q12" s="72"/>
-      <c r="R12" s="72"/>
-      <c r="S12" s="72"/>
-      <c r="T12" s="72"/>
-      <c r="U12" s="72"/>
-      <c r="V12" s="72"/>
-      <c r="W12" s="72"/>
-      <c r="X12" s="72"/>
-      <c r="Y12" s="72"/>
-      <c r="Z12" s="72"/>
-      <c r="AA12" s="73"/>
+      <c r="D12" s="75"/>
+      <c r="E12" s="75"/>
+      <c r="F12" s="75"/>
+      <c r="G12" s="75"/>
+      <c r="H12" s="75"/>
+      <c r="I12" s="75"/>
+      <c r="J12" s="75"/>
+      <c r="K12" s="75"/>
+      <c r="L12" s="75"/>
+      <c r="M12" s="75"/>
+      <c r="N12" s="75"/>
+      <c r="O12" s="75"/>
+      <c r="P12" s="75"/>
+      <c r="Q12" s="75"/>
+      <c r="R12" s="75"/>
+      <c r="S12" s="75"/>
+      <c r="T12" s="75"/>
+      <c r="U12" s="75"/>
+      <c r="V12" s="75"/>
+      <c r="W12" s="75"/>
+      <c r="X12" s="75"/>
+      <c r="Y12" s="75"/>
+      <c r="Z12" s="75"/>
+      <c r="AA12" s="76"/>
       <c r="AB12" s="12"/>
       <c r="AC12" s="13" t="s">
         <v>4</v>
@@ -2270,21 +2276,21 @@
       <c r="U13" s="22"/>
       <c r="V13" s="22"/>
       <c r="W13" s="12"/>
-      <c r="X13" s="77" t="s">
+      <c r="X13" s="78" t="s">
         <v>12</v>
       </c>
-      <c r="Y13" s="78"/>
-      <c r="Z13" s="77" t="s">
+      <c r="Y13" s="79"/>
+      <c r="Z13" s="78" t="s">
         <v>13</v>
       </c>
-      <c r="AA13" s="79"/>
+      <c r="AA13" s="80"/>
       <c r="AB13" s="23"/>
       <c r="AC13" s="24"/>
-      <c r="AD13" s="75" t="s">
-        <v>70</v>
-      </c>
-      <c r="AE13" s="80"/>
-      <c r="AF13" s="76"/>
+      <c r="AD13" s="71" t="s">
+        <v>69</v>
+      </c>
+      <c r="AE13" s="72"/>
+      <c r="AF13" s="73"/>
       <c r="AG13" s="25"/>
       <c r="AH13" s="26"/>
       <c r="AI13" s="20"/>
@@ -2295,7 +2301,7 @@
       <c r="AN13" s="4"/>
       <c r="AO13" s="4"/>
     </row>
-    <row r="14" spans="1:42" ht="30" customHeight="1">
+    <row r="14" spans="1:42" ht="131.4" customHeight="1">
       <c r="A14" s="10"/>
       <c r="B14" s="11"/>
       <c r="C14" s="19"/>
@@ -2326,19 +2332,19 @@
       <c r="AB14" s="32"/>
       <c r="AC14" s="33"/>
       <c r="AD14" s="34" t="s">
+        <v>47</v>
+      </c>
+      <c r="AE14" s="34" t="s">
         <v>48</v>
       </c>
-      <c r="AE14" s="34" t="s">
+      <c r="AF14" s="34" t="s">
         <v>49</v>
       </c>
-      <c r="AF14" s="34" t="s">
-        <v>50</v>
-      </c>
       <c r="AG14" s="35" t="s">
+        <v>70</v>
+      </c>
+      <c r="AH14" s="36" t="s">
         <v>71</v>
-      </c>
-      <c r="AH14" s="36" t="s">
-        <v>16</v>
       </c>
       <c r="AI14" s="20"/>
       <c r="AJ14" s="20"/>
@@ -2352,7 +2358,7 @@
       <c r="A15" s="37"/>
       <c r="B15" s="38"/>
       <c r="C15" s="39" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D15" s="40"/>
       <c r="E15" s="40"/>
@@ -2365,7 +2371,7 @@
       <c r="L15" s="40"/>
       <c r="M15" s="40"/>
       <c r="N15" s="39" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="O15" s="40"/>
       <c r="P15" s="40"/>
@@ -2374,57 +2380,57 @@
       <c r="S15" s="40"/>
       <c r="T15" s="40"/>
       <c r="U15" s="41" t="s">
+        <v>18</v>
+      </c>
+      <c r="V15" s="41" t="s">
         <v>19</v>
-      </c>
-      <c r="V15" s="41" t="s">
-        <v>20</v>
       </c>
       <c r="W15" s="42"/>
       <c r="X15" s="43" t="s">
+        <v>20</v>
+      </c>
+      <c r="Y15" s="44" t="s">
         <v>21</v>
       </c>
-      <c r="Y15" s="44" t="s">
+      <c r="Z15" s="45" t="s">
         <v>22</v>
       </c>
-      <c r="Z15" s="45" t="s">
+      <c r="AA15" s="46" t="s">
         <v>23</v>
-      </c>
-      <c r="AA15" s="46" t="s">
-        <v>24</v>
       </c>
       <c r="AB15" s="47"/>
       <c r="AC15" s="48" t="s">
+        <v>24</v>
+      </c>
+      <c r="AD15" s="49" t="s">
         <v>25</v>
       </c>
-      <c r="AD15" s="49" t="s">
+      <c r="AE15" s="49" t="s">
         <v>26</v>
       </c>
-      <c r="AE15" s="49" t="s">
+      <c r="AF15" s="49" t="s">
+        <v>50</v>
+      </c>
+      <c r="AG15" s="50" t="s">
         <v>27</v>
       </c>
-      <c r="AF15" s="49" t="s">
-        <v>51</v>
-      </c>
-      <c r="AG15" s="50" t="s">
+      <c r="AH15" s="50" t="s">
         <v>28</v>
       </c>
-      <c r="AH15" s="50" t="s">
+      <c r="AI15" s="51" t="s">
         <v>29</v>
       </c>
-      <c r="AI15" s="51" t="s">
+      <c r="AJ15" s="52" t="s">
         <v>30</v>
       </c>
-      <c r="AJ15" s="52" t="s">
+      <c r="AK15" s="52" t="s">
         <v>31</v>
       </c>
-      <c r="AK15" s="52" t="s">
+      <c r="AL15" s="52" t="s">
         <v>32</v>
       </c>
-      <c r="AL15" s="52" t="s">
+      <c r="AM15" s="51" t="s">
         <v>33</v>
-      </c>
-      <c r="AM15" s="51" t="s">
-        <v>34</v>
       </c>
       <c r="AN15" s="3"/>
       <c r="AO15" s="3"/>
@@ -2446,7 +2452,7 @@
       <c r="L16" s="65"/>
       <c r="M16" s="65"/>
       <c r="N16" s="66" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="O16" s="67"/>
       <c r="P16" s="67"/>
@@ -2455,59 +2461,59 @@
       <c r="S16" s="67"/>
       <c r="T16" s="67"/>
       <c r="U16" s="67" t="str">
-        <f t="shared" ref="U16:U18" si="6">N16</f>
+        <f t="shared" ref="U16:U18" si="5">N16</f>
         <v>email</v>
       </c>
       <c r="V16" s="67" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="W16" s="57"/>
       <c r="X16" s="58" t="s">
+        <v>53</v>
+      </c>
+      <c r="Y16" s="58" t="s">
         <v>54</v>
       </c>
-      <c r="Y16" s="58" t="s">
+      <c r="Z16" s="58" t="s">
         <v>55</v>
       </c>
-      <c r="Z16" s="58" t="s">
+      <c r="AA16" s="58" t="s">
         <v>56</v>
-      </c>
-      <c r="AA16" s="58" t="s">
-        <v>57</v>
       </c>
       <c r="AB16" s="59"/>
       <c r="AC16" s="60" t="str">
-        <f t="shared" ref="AC16:AC18" si="7">X16</f>
+        <f t="shared" ref="AC16:AC18" si="6">X16</f>
         <v>Person's email cannot be null</v>
       </c>
       <c r="AD16" s="61" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="AE16" s="68"/>
       <c r="AF16" s="61"/>
       <c r="AG16" s="62" t="str">
-        <f t="shared" ref="AG16:AG18" si="8">CONCATENATE( "person",",",U16,",",$X$6,",",C16," [",U16,"] - ",X16,",",X16,",",Y16,",", $Z$6,",",C16," [",U16,"] - ",Z16,",",Z16,",",AA16,",","$person.getEmail()")</f>
+        <f>CONCATENATE( "person",",",U16,",",$X$6,",",C16," [",U16,"] - ",X16,",",X16,",",Y16,",", $Z$6,",",C16," [",U16,"] - ",Z16,",",Z16,",",AA16,",","$person.getEmail()")</f>
         <v>person,email,en,2 [email] - Person's email cannot be null,Person's email cannot be null,An email with some value different than null,es,2 [email] - El email de la persona no puede ser nulo,El email de la persona no puede ser nulo,Un email con algún valor diferente de nulo,$person.getEmail()</v>
       </c>
       <c r="AH16" s="58" t="str">
-        <f t="shared" ref="AH16:AH18" si="9">CONCATENATE("ERROR",",",X16)</f>
+        <f t="shared" ref="AH16:AH18" si="7">CONCATENATE("ERROR",",",X16)</f>
         <v>ERROR,Person's email cannot be null</v>
       </c>
       <c r="AI16" s="63" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="AJ16" s="64" t="str">
-        <f t="shared" ref="AJ16:AJ18" si="10">U16</f>
+        <f t="shared" ref="AJ16:AJ18" si="8">U16</f>
         <v>email</v>
       </c>
       <c r="AK16" s="64">
         <v>100</v>
       </c>
       <c r="AL16" s="63" t="str">
-        <f t="shared" ref="AL16:AL18" si="11">IF(AD16="COMPLETE","false","true")</f>
+        <f t="shared" ref="AL16:AL18" si="9">IF(AD16="COMPLETE","false","true")</f>
         <v>true</v>
       </c>
       <c r="AM16" s="63" t="str">
-        <f t="shared" ref="AM16:AM18" si="12">IF(AC16="COMPLETE","false","true")</f>
+        <f t="shared" ref="AM16:AM18" si="10">IF(AC16="COMPLETE","false","true")</f>
         <v>true</v>
       </c>
       <c r="AN16" s="4"/>
@@ -2530,7 +2536,7 @@
       <c r="L17" s="65"/>
       <c r="M17" s="65"/>
       <c r="N17" s="66" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="O17" s="67"/>
       <c r="P17" s="67"/>
@@ -2539,65 +2545,65 @@
       <c r="S17" s="67"/>
       <c r="T17" s="67"/>
       <c r="U17" s="67" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>email</v>
       </c>
       <c r="V17" s="67" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="W17" s="57"/>
       <c r="X17" s="58" t="s">
+        <v>57</v>
+      </c>
+      <c r="Y17" s="58" t="s">
         <v>58</v>
       </c>
-      <c r="Y17" s="58" t="s">
+      <c r="Z17" s="58" t="s">
         <v>59</v>
       </c>
-      <c r="Z17" s="58" t="s">
+      <c r="AA17" s="58" t="s">
         <v>60</v>
-      </c>
-      <c r="AA17" s="58" t="s">
-        <v>61</v>
       </c>
       <c r="AB17" s="59"/>
       <c r="AC17" s="60" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>Person's email cannot be empty</v>
       </c>
       <c r="AD17" s="64"/>
       <c r="AE17" s="61" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="AF17" s="69"/>
       <c r="AG17" s="62" t="str">
+        <f t="shared" ref="AG17:AG18" si="11">CONCATENATE( "person",",",U17,",",$X$6,",",C17," [",U17,"] - ",X17,",",X17,",",Y17,",", $Z$6,",",C17," [",U17,"] - ",Z17,",",Z17,",",AA17,",","$person.getEmail()")</f>
+        <v>person,email,en,2 [email] - Person's email cannot be empty,Person's email cannot be empty,An email with some value different than empty,es,2 [email] - El email de la persona no puede ser vacío,El email de la persona no puede ser vacío,Un email con algún valor diferente de vacío,$person.getEmail()</v>
+      </c>
+      <c r="AH17" s="58" t="str">
+        <f t="shared" si="7"/>
+        <v>ERROR,Person's email cannot be empty</v>
+      </c>
+      <c r="AI17" s="63" t="s">
+        <v>41</v>
+      </c>
+      <c r="AJ17" s="64" t="str">
         <f t="shared" si="8"/>
-        <v>person,email,en,2 [email] - Person's email cannot be empty,Person's email cannot be empty,An email with some value different than empty,es,2 [email] - El email de la persona no puede ser vacío,El email de la persona no puede ser vacío,Un email con algún valor diferente de vacío,$person.getEmail()</v>
-      </c>
-      <c r="AH17" s="58" t="str">
-        <f t="shared" si="9"/>
-        <v>ERROR,Person's email cannot be empty</v>
-      </c>
-      <c r="AI17" s="63" t="s">
-        <v>42</v>
-      </c>
-      <c r="AJ17" s="64" t="str">
-        <f t="shared" si="10"/>
         <v>email</v>
       </c>
       <c r="AK17" s="64">
         <v>99</v>
       </c>
       <c r="AL17" s="63" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>true</v>
       </c>
       <c r="AM17" s="63" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>true</v>
       </c>
       <c r="AN17" s="4"/>
       <c r="AO17" s="4"/>
     </row>
-    <row r="18" spans="1:41" ht="72">
+    <row r="18" spans="1:41" ht="86.4">
       <c r="A18" s="4"/>
       <c r="B18" s="53"/>
       <c r="C18" s="65">
@@ -2614,7 +2620,7 @@
       <c r="L18" s="65"/>
       <c r="M18" s="65"/>
       <c r="N18" s="66" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="O18" s="67"/>
       <c r="P18" s="67"/>
@@ -2623,59 +2629,59 @@
       <c r="S18" s="67"/>
       <c r="T18" s="67"/>
       <c r="U18" s="67" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>email</v>
       </c>
       <c r="V18" s="67" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="W18" s="57"/>
       <c r="X18" s="60" t="s">
+        <v>61</v>
+      </c>
+      <c r="Y18" s="60" t="s">
         <v>62</v>
       </c>
-      <c r="Y18" s="60" t="s">
+      <c r="Z18" s="60" t="s">
         <v>63</v>
       </c>
-      <c r="Z18" s="60" t="s">
+      <c r="AA18" s="60" t="s">
         <v>64</v>
-      </c>
-      <c r="AA18" s="60" t="s">
-        <v>65</v>
       </c>
       <c r="AB18" s="59"/>
       <c r="AC18" s="60" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>Person's email is not valid</v>
       </c>
       <c r="AD18" s="64"/>
       <c r="AE18" s="64"/>
       <c r="AF18" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="AG18" s="62" t="str">
+        <f t="shared" si="11"/>
+        <v>person,email,en,2 [email] - Person's email is not valid,Person's email is not valid,A valid email,es,2 [email] - El email de la persona es incorrecto,El email de la persona es incorrecto,Un email válido,$person.getEmail()</v>
+      </c>
+      <c r="AH18" s="58" t="str">
+        <f t="shared" si="7"/>
+        <v>ERROR,Person's email is not valid</v>
+      </c>
+      <c r="AI18" s="63" t="s">
         <v>66</v>
       </c>
-      <c r="AG18" s="62" t="str">
+      <c r="AJ18" s="64" t="str">
         <f t="shared" si="8"/>
-        <v>person,email,en,2 [email] - Person's email is not valid,Person's email is not valid,A valid email,es,2 [email] - El email de la persona es incorrecto,El email de la persona es incorrecto,Un email válido,$person.getEmail()</v>
-      </c>
-      <c r="AH18" s="58" t="str">
-        <f t="shared" si="9"/>
-        <v>ERROR,Person's email is not valid</v>
-      </c>
-      <c r="AI18" s="63" t="s">
-        <v>67</v>
-      </c>
-      <c r="AJ18" s="64" t="str">
-        <f t="shared" si="10"/>
         <v>email</v>
       </c>
       <c r="AK18" s="64">
         <v>98</v>
       </c>
       <c r="AL18" s="63" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>true</v>
       </c>
       <c r="AM18" s="63" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>true</v>
       </c>
       <c r="AN18" s="4"/>
@@ -3663,16 +3669,16 @@
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B4:AL4"/>
+    <mergeCell ref="C5:AA5"/>
+    <mergeCell ref="AD6:AE6"/>
+    <mergeCell ref="X6:Y6"/>
+    <mergeCell ref="Z6:AA6"/>
     <mergeCell ref="AD13:AF13"/>
     <mergeCell ref="B11:AM11"/>
     <mergeCell ref="C12:AA12"/>
     <mergeCell ref="X13:Y13"/>
     <mergeCell ref="Z13:AA13"/>
-    <mergeCell ref="B4:AL4"/>
-    <mergeCell ref="C5:AA5"/>
-    <mergeCell ref="AD6:AE6"/>
-    <mergeCell ref="X6:Y6"/>
-    <mergeCell ref="Z6:AA6"/>
   </mergeCells>
   <conditionalFormatting sqref="W1:W3">
     <cfRule type="cellIs" dxfId="27" priority="1" operator="equal">

</xml_diff>

<commit_message>
Migrating storage to mongo
</commit_message>
<xml_diff>
--- a/src/test/resources/rules.xlsx
+++ b/src/test/resources/rules.xlsx
@@ -973,11 +973,9 @@
     <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -986,14 +984,16 @@
     <xf numFmtId="0" fontId="8" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1501,25 +1501,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AP1000"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="AD15" workbookViewId="0">
-      <selection activeCell="AG16" sqref="AG16:AG18"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="AD16" workbookViewId="0">
+      <selection activeCell="AG19" sqref="AG19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="2.33203125" customWidth="1"/>
     <col min="2" max="2" width="0.88671875" customWidth="1"/>
-    <col min="3" max="3" width="2.44140625" style="80" customWidth="1"/>
-    <col min="4" max="4" width="1" style="80" customWidth="1"/>
-    <col min="5" max="5" width="1.88671875" style="80" customWidth="1"/>
-    <col min="6" max="6" width="0.5546875" style="80" customWidth="1"/>
-    <col min="7" max="7" width="1.88671875" style="80" customWidth="1"/>
-    <col min="8" max="8" width="0.5546875" style="80" customWidth="1"/>
-    <col min="9" max="9" width="1.88671875" style="80" customWidth="1"/>
-    <col min="10" max="10" width="0.5546875" style="80" customWidth="1"/>
-    <col min="11" max="11" width="1.88671875" style="80" customWidth="1"/>
-    <col min="12" max="12" width="0.5546875" style="80" customWidth="1"/>
-    <col min="13" max="13" width="1.88671875" style="80" customWidth="1"/>
+    <col min="3" max="3" width="2.44140625" style="70" customWidth="1"/>
+    <col min="4" max="4" width="1" style="70" customWidth="1"/>
+    <col min="5" max="5" width="1.88671875" style="70" customWidth="1"/>
+    <col min="6" max="6" width="0.5546875" style="70" customWidth="1"/>
+    <col min="7" max="7" width="1.88671875" style="70" customWidth="1"/>
+    <col min="8" max="8" width="0.5546875" style="70" customWidth="1"/>
+    <col min="9" max="9" width="1.88671875" style="70" customWidth="1"/>
+    <col min="10" max="10" width="0.5546875" style="70" customWidth="1"/>
+    <col min="11" max="11" width="1.88671875" style="70" customWidth="1"/>
+    <col min="12" max="12" width="0.5546875" style="70" customWidth="1"/>
+    <col min="13" max="13" width="1.88671875" style="70" customWidth="1"/>
     <col min="14" max="20" width="2" customWidth="1"/>
     <col min="21" max="21" width="22.5546875" customWidth="1"/>
     <col min="22" max="22" width="33.109375" customWidth="1"/>
@@ -1683,45 +1683,45 @@
     </row>
     <row r="4" spans="1:42" ht="21">
       <c r="A4" s="3"/>
-      <c r="B4" s="73" t="s">
+      <c r="B4" s="71" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="74"/>
-      <c r="D4" s="74"/>
-      <c r="E4" s="74"/>
-      <c r="F4" s="74"/>
-      <c r="G4" s="74"/>
-      <c r="H4" s="74"/>
-      <c r="I4" s="74"/>
-      <c r="J4" s="74"/>
-      <c r="K4" s="74"/>
-      <c r="L4" s="74"/>
-      <c r="M4" s="74"/>
-      <c r="N4" s="74"/>
-      <c r="O4" s="74"/>
-      <c r="P4" s="74"/>
-      <c r="Q4" s="74"/>
-      <c r="R4" s="74"/>
-      <c r="S4" s="74"/>
-      <c r="T4" s="74"/>
-      <c r="U4" s="74"/>
-      <c r="V4" s="74"/>
-      <c r="W4" s="74"/>
-      <c r="X4" s="74"/>
-      <c r="Y4" s="74"/>
-      <c r="Z4" s="74"/>
-      <c r="AA4" s="74"/>
-      <c r="AB4" s="74"/>
-      <c r="AC4" s="74"/>
-      <c r="AD4" s="74"/>
-      <c r="AE4" s="74"/>
-      <c r="AF4" s="74"/>
-      <c r="AG4" s="74"/>
-      <c r="AH4" s="74"/>
-      <c r="AI4" s="74"/>
-      <c r="AJ4" s="74"/>
-      <c r="AK4" s="74"/>
-      <c r="AL4" s="75"/>
+      <c r="C4" s="72"/>
+      <c r="D4" s="72"/>
+      <c r="E4" s="72"/>
+      <c r="F4" s="72"/>
+      <c r="G4" s="72"/>
+      <c r="H4" s="72"/>
+      <c r="I4" s="72"/>
+      <c r="J4" s="72"/>
+      <c r="K4" s="72"/>
+      <c r="L4" s="72"/>
+      <c r="M4" s="72"/>
+      <c r="N4" s="72"/>
+      <c r="O4" s="72"/>
+      <c r="P4" s="72"/>
+      <c r="Q4" s="72"/>
+      <c r="R4" s="72"/>
+      <c r="S4" s="72"/>
+      <c r="T4" s="72"/>
+      <c r="U4" s="72"/>
+      <c r="V4" s="72"/>
+      <c r="W4" s="72"/>
+      <c r="X4" s="72"/>
+      <c r="Y4" s="72"/>
+      <c r="Z4" s="72"/>
+      <c r="AA4" s="72"/>
+      <c r="AB4" s="72"/>
+      <c r="AC4" s="72"/>
+      <c r="AD4" s="72"/>
+      <c r="AE4" s="72"/>
+      <c r="AF4" s="72"/>
+      <c r="AG4" s="72"/>
+      <c r="AH4" s="72"/>
+      <c r="AI4" s="72"/>
+      <c r="AJ4" s="72"/>
+      <c r="AK4" s="72"/>
+      <c r="AL4" s="73"/>
       <c r="AM4" s="3"/>
       <c r="AN4" s="3"/>
       <c r="AO4" s="3"/>
@@ -1729,33 +1729,33 @@
     <row r="5" spans="1:42" ht="15" customHeight="1">
       <c r="A5" s="10"/>
       <c r="B5" s="11"/>
-      <c r="C5" s="76" t="s">
+      <c r="C5" s="74" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="74"/>
-      <c r="E5" s="74"/>
-      <c r="F5" s="74"/>
-      <c r="G5" s="74"/>
-      <c r="H5" s="74"/>
-      <c r="I5" s="74"/>
-      <c r="J5" s="74"/>
-      <c r="K5" s="74"/>
-      <c r="L5" s="74"/>
-      <c r="M5" s="74"/>
-      <c r="N5" s="74"/>
-      <c r="O5" s="74"/>
-      <c r="P5" s="74"/>
-      <c r="Q5" s="74"/>
-      <c r="R5" s="74"/>
-      <c r="S5" s="74"/>
-      <c r="T5" s="74"/>
-      <c r="U5" s="74"/>
-      <c r="V5" s="74"/>
-      <c r="W5" s="74"/>
-      <c r="X5" s="74"/>
-      <c r="Y5" s="74"/>
-      <c r="Z5" s="74"/>
-      <c r="AA5" s="75"/>
+      <c r="D5" s="72"/>
+      <c r="E5" s="72"/>
+      <c r="F5" s="72"/>
+      <c r="G5" s="72"/>
+      <c r="H5" s="72"/>
+      <c r="I5" s="72"/>
+      <c r="J5" s="72"/>
+      <c r="K5" s="72"/>
+      <c r="L5" s="72"/>
+      <c r="M5" s="72"/>
+      <c r="N5" s="72"/>
+      <c r="O5" s="72"/>
+      <c r="P5" s="72"/>
+      <c r="Q5" s="72"/>
+      <c r="R5" s="72"/>
+      <c r="S5" s="72"/>
+      <c r="T5" s="72"/>
+      <c r="U5" s="72"/>
+      <c r="V5" s="72"/>
+      <c r="W5" s="72"/>
+      <c r="X5" s="72"/>
+      <c r="Y5" s="72"/>
+      <c r="Z5" s="72"/>
+      <c r="AA5" s="73"/>
       <c r="AB5" s="12"/>
       <c r="AC5" s="13" t="s">
         <v>4</v>
@@ -1825,10 +1825,10 @@
       <c r="AA6" s="79"/>
       <c r="AB6" s="22"/>
       <c r="AC6" s="23"/>
-      <c r="AD6" s="70" t="s">
+      <c r="AD6" s="75" t="s">
         <v>69</v>
       </c>
-      <c r="AE6" s="72"/>
+      <c r="AE6" s="76"/>
       <c r="AF6" s="24"/>
       <c r="AG6" s="25"/>
       <c r="AH6" s="19"/>
@@ -2147,79 +2147,79 @@
     </row>
     <row r="11" spans="1:42" ht="21">
       <c r="A11" s="3"/>
-      <c r="B11" s="73" t="s">
+      <c r="B11" s="71" t="s">
         <v>46</v>
       </c>
-      <c r="C11" s="74"/>
-      <c r="D11" s="74"/>
-      <c r="E11" s="74"/>
-      <c r="F11" s="74"/>
-      <c r="G11" s="74"/>
-      <c r="H11" s="74"/>
-      <c r="I11" s="74"/>
-      <c r="J11" s="74"/>
-      <c r="K11" s="74"/>
-      <c r="L11" s="74"/>
-      <c r="M11" s="74"/>
-      <c r="N11" s="74"/>
-      <c r="O11" s="74"/>
-      <c r="P11" s="74"/>
-      <c r="Q11" s="74"/>
-      <c r="R11" s="74"/>
-      <c r="S11" s="74"/>
-      <c r="T11" s="74"/>
-      <c r="U11" s="74"/>
-      <c r="V11" s="74"/>
-      <c r="W11" s="74"/>
-      <c r="X11" s="74"/>
-      <c r="Y11" s="74"/>
-      <c r="Z11" s="74"/>
-      <c r="AA11" s="74"/>
-      <c r="AB11" s="74"/>
-      <c r="AC11" s="74"/>
-      <c r="AD11" s="74"/>
-      <c r="AE11" s="74"/>
-      <c r="AF11" s="74"/>
-      <c r="AG11" s="74"/>
-      <c r="AH11" s="74"/>
-      <c r="AI11" s="74"/>
-      <c r="AJ11" s="74"/>
-      <c r="AK11" s="74"/>
-      <c r="AL11" s="74"/>
-      <c r="AM11" s="75"/>
+      <c r="C11" s="72"/>
+      <c r="D11" s="72"/>
+      <c r="E11" s="72"/>
+      <c r="F11" s="72"/>
+      <c r="G11" s="72"/>
+      <c r="H11" s="72"/>
+      <c r="I11" s="72"/>
+      <c r="J11" s="72"/>
+      <c r="K11" s="72"/>
+      <c r="L11" s="72"/>
+      <c r="M11" s="72"/>
+      <c r="N11" s="72"/>
+      <c r="O11" s="72"/>
+      <c r="P11" s="72"/>
+      <c r="Q11" s="72"/>
+      <c r="R11" s="72"/>
+      <c r="S11" s="72"/>
+      <c r="T11" s="72"/>
+      <c r="U11" s="72"/>
+      <c r="V11" s="72"/>
+      <c r="W11" s="72"/>
+      <c r="X11" s="72"/>
+      <c r="Y11" s="72"/>
+      <c r="Z11" s="72"/>
+      <c r="AA11" s="72"/>
+      <c r="AB11" s="72"/>
+      <c r="AC11" s="72"/>
+      <c r="AD11" s="72"/>
+      <c r="AE11" s="72"/>
+      <c r="AF11" s="72"/>
+      <c r="AG11" s="72"/>
+      <c r="AH11" s="72"/>
+      <c r="AI11" s="72"/>
+      <c r="AJ11" s="72"/>
+      <c r="AK11" s="72"/>
+      <c r="AL11" s="72"/>
+      <c r="AM11" s="73"/>
       <c r="AN11" s="3"/>
       <c r="AO11" s="3"/>
     </row>
     <row r="12" spans="1:42" ht="15" customHeight="1">
       <c r="A12" s="10"/>
       <c r="B12" s="11"/>
-      <c r="C12" s="76" t="s">
+      <c r="C12" s="74" t="s">
         <v>3</v>
       </c>
-      <c r="D12" s="74"/>
-      <c r="E12" s="74"/>
-      <c r="F12" s="74"/>
-      <c r="G12" s="74"/>
-      <c r="H12" s="74"/>
-      <c r="I12" s="74"/>
-      <c r="J12" s="74"/>
-      <c r="K12" s="74"/>
-      <c r="L12" s="74"/>
-      <c r="M12" s="74"/>
-      <c r="N12" s="74"/>
-      <c r="O12" s="74"/>
-      <c r="P12" s="74"/>
-      <c r="Q12" s="74"/>
-      <c r="R12" s="74"/>
-      <c r="S12" s="74"/>
-      <c r="T12" s="74"/>
-      <c r="U12" s="74"/>
-      <c r="V12" s="74"/>
-      <c r="W12" s="74"/>
-      <c r="X12" s="74"/>
-      <c r="Y12" s="74"/>
-      <c r="Z12" s="74"/>
-      <c r="AA12" s="75"/>
+      <c r="D12" s="72"/>
+      <c r="E12" s="72"/>
+      <c r="F12" s="72"/>
+      <c r="G12" s="72"/>
+      <c r="H12" s="72"/>
+      <c r="I12" s="72"/>
+      <c r="J12" s="72"/>
+      <c r="K12" s="72"/>
+      <c r="L12" s="72"/>
+      <c r="M12" s="72"/>
+      <c r="N12" s="72"/>
+      <c r="O12" s="72"/>
+      <c r="P12" s="72"/>
+      <c r="Q12" s="72"/>
+      <c r="R12" s="72"/>
+      <c r="S12" s="72"/>
+      <c r="T12" s="72"/>
+      <c r="U12" s="72"/>
+      <c r="V12" s="72"/>
+      <c r="W12" s="72"/>
+      <c r="X12" s="72"/>
+      <c r="Y12" s="72"/>
+      <c r="Z12" s="72"/>
+      <c r="AA12" s="73"/>
       <c r="AB12" s="12"/>
       <c r="AC12" s="13" t="s">
         <v>4</v>
@@ -2291,11 +2291,11 @@
       <c r="AA13" s="79"/>
       <c r="AB13" s="22"/>
       <c r="AC13" s="23"/>
-      <c r="AD13" s="70" t="s">
+      <c r="AD13" s="75" t="s">
         <v>69</v>
       </c>
-      <c r="AE13" s="71"/>
-      <c r="AF13" s="72"/>
+      <c r="AE13" s="80"/>
+      <c r="AF13" s="76"/>
       <c r="AG13" s="24"/>
       <c r="AH13" s="25"/>
       <c r="AI13" s="19"/>
@@ -2616,7 +2616,7 @@
       <c r="AN17" s="4"/>
       <c r="AO17" s="4"/>
     </row>
-    <row r="18" spans="1:41" ht="115.2">
+    <row r="18" spans="1:41" ht="86.4">
       <c r="A18" s="4"/>
       <c r="B18" s="52"/>
       <c r="C18" s="64">
@@ -3686,16 +3686,16 @@
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="AD13:AF13"/>
+    <mergeCell ref="B11:AM11"/>
+    <mergeCell ref="C12:AA12"/>
+    <mergeCell ref="X13:Y13"/>
+    <mergeCell ref="Z13:AA13"/>
     <mergeCell ref="B4:AL4"/>
     <mergeCell ref="C5:AA5"/>
     <mergeCell ref="AD6:AE6"/>
     <mergeCell ref="X6:Y6"/>
     <mergeCell ref="Z6:AA6"/>
-    <mergeCell ref="AD13:AF13"/>
-    <mergeCell ref="B11:AM11"/>
-    <mergeCell ref="C12:AA12"/>
-    <mergeCell ref="X13:Y13"/>
-    <mergeCell ref="Z13:AA13"/>
   </mergeCells>
   <conditionalFormatting sqref="W1:W3">
     <cfRule type="cellIs" dxfId="27" priority="1" operator="equal">

</xml_diff>